<commit_message>
added one peptide to FP-sum
</commit_message>
<xml_diff>
--- a/Kd_FP_sum.xlsx
+++ b/Kd_FP_sum.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\D disc\GG LAB\pdz_ms project\ms_manuscripts\figure5_FpVsMs-plot\matlab\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\D disc\GG LAB\pdz_ms project\ms-peptide-kd\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E22232B4-1E98-4A38-8870-2413A9491671}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9485778E-66AE-4E8E-98D1-6457AF2F9DE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B8A6AFAB-7115-4F3B-8AAB-1B272927A5B0}"/>
+    <workbookView xWindow="3384" yWindow="3384" windowWidth="17280" windowHeight="8964" xr2:uid="{B8A6AFAB-7115-4F3B-8AAB-1B272927A5B0}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet1" sheetId="8" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="37">
   <si>
     <t>FFSTRL</t>
   </si>
@@ -142,6 +142,9 @@
   </si>
   <si>
     <t>APMKWL</t>
+  </si>
+  <si>
+    <t>DFATTV</t>
   </si>
 </sst>
 </file>
@@ -261,7 +264,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -293,12 +296,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -327,6 +324,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -643,10 +643,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC4613C4-1397-45B2-8CD1-6BCB538DECD7}">
-  <dimension ref="A1:D36"/>
+  <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37:C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -707,7 +707,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="17" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="2">
@@ -718,7 +718,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="17" t="s">
         <v>0</v>
       </c>
       <c r="B7" s="6">
@@ -729,7 +729,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="19" t="s">
+      <c r="A8" s="17" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="2">
@@ -740,7 +740,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="17" t="s">
+      <c r="A9" s="15" t="s">
         <v>19</v>
       </c>
       <c r="B9" s="2">
@@ -751,7 +751,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="17" t="s">
+      <c r="A10" s="15" t="s">
         <v>20</v>
       </c>
       <c r="B10" s="2">
@@ -762,7 +762,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="19" t="s">
+      <c r="A11" s="17" t="s">
         <v>2</v>
       </c>
       <c r="B11" s="2">
@@ -773,7 +773,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="17" t="s">
+      <c r="A12" s="15" t="s">
         <v>21</v>
       </c>
       <c r="B12" s="2">
@@ -784,29 +784,29 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="14" t="s">
+      <c r="A13" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="13">
+      <c r="B13" s="11">
         <v>10.45</v>
       </c>
-      <c r="C13" s="13">
+      <c r="C13" s="11">
         <v>1.86</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="14" t="s">
+      <c r="A14" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="13">
+      <c r="B14" s="11">
         <v>11.57</v>
       </c>
-      <c r="C14" s="13">
+      <c r="C14" s="11">
         <v>0.27</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="19" t="s">
+      <c r="A15" s="17" t="s">
         <v>5</v>
       </c>
       <c r="B15" s="2">
@@ -817,35 +817,35 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="14" t="s">
+      <c r="A16" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="15">
+      <c r="B16" s="13">
         <v>20.54</v>
       </c>
-      <c r="C16" s="13">
+      <c r="C16" s="11">
         <v>5.55</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="20" t="s">
+      <c r="A17" s="18" t="s">
         <v>16</v>
       </c>
       <c r="B17" s="7">
         <v>25.24</v>
       </c>
-      <c r="C17" s="22">
+      <c r="C17" s="20">
         <v>1.29</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="16" t="s">
+      <c r="A18" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="B18" s="13">
+      <c r="B18" s="11">
         <v>26.3</v>
       </c>
-      <c r="C18" s="13">
+      <c r="C18" s="11">
         <v>4.43</v>
       </c>
     </row>
@@ -861,13 +861,13 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="16" t="s">
+      <c r="A20" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B20" s="15">
+      <c r="B20" s="13">
         <v>35.83</v>
       </c>
-      <c r="C20" s="13">
+      <c r="C20" s="11">
         <v>4.75</v>
       </c>
     </row>
@@ -894,24 +894,24 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="16" t="s">
+      <c r="A23" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="B23" s="15">
+      <c r="B23" s="13">
         <v>51.66</v>
       </c>
-      <c r="C23" s="13">
+      <c r="C23" s="11">
         <v>2.69</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="16" t="s">
+      <c r="A24" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="B24" s="21">
+      <c r="B24" s="19">
         <v>53.27</v>
       </c>
-      <c r="C24" s="21">
+      <c r="C24" s="19">
         <v>4.12</v>
       </c>
     </row>
@@ -927,7 +927,7 @@
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="18" t="s">
+      <c r="A26" s="16" t="s">
         <v>34</v>
       </c>
       <c r="B26" s="3">
@@ -941,13 +941,13 @@
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="16" t="s">
+      <c r="A27" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="B27" s="13">
+      <c r="B27" s="11">
         <v>75.510000000000005</v>
       </c>
-      <c r="C27" s="13">
+      <c r="C27" s="11">
         <v>10.27</v>
       </c>
     </row>
@@ -966,24 +966,24 @@
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" s="16" t="s">
+      <c r="A29" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="13">
+      <c r="B29" s="11">
         <v>83.17</v>
       </c>
-      <c r="C29" s="13">
+      <c r="C29" s="11">
         <v>4.99</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="16" t="s">
+      <c r="A30" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="B30" s="13">
+      <c r="B30" s="11">
         <v>83.9</v>
       </c>
-      <c r="C30" s="13">
+      <c r="C30" s="11">
         <v>10.44</v>
       </c>
     </row>
@@ -1010,13 +1010,13 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="16" t="s">
+      <c r="A33" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="B33" s="13">
+      <c r="B33" s="11">
         <v>160.76</v>
       </c>
-      <c r="C33" s="13">
+      <c r="C33" s="11">
         <v>12.45</v>
       </c>
       <c r="D33" t="s">
@@ -1024,13 +1024,13 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" s="16" t="s">
+      <c r="A34" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="B34" s="13">
+      <c r="B34" s="11">
         <v>309.85000000000002</v>
       </c>
-      <c r="C34" s="13">
+      <c r="C34" s="11">
         <v>46.3</v>
       </c>
       <c r="D34" t="s">
@@ -1038,14 +1038,23 @@
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" s="18"/>
-      <c r="B35" s="11"/>
-      <c r="C35" s="12"/>
+      <c r="A35" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="B35">
+        <v>108.76</v>
+      </c>
+      <c r="C35">
+        <v>9.6199999999999992</v>
+      </c>
     </row>
     <row r="36" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="10"/>
       <c r="B36" s="2"/>
       <c r="C36" s="6"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" s="21"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C37">

</xml_diff>